<commit_message>
refactorings. First PoC of a comparative report
</commit_message>
<xml_diff>
--- a/test_configs.xlsx
+++ b/test_configs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Purpose of this file:</t>
   </si>
@@ -69,38 +69,26 @@
     <t>con.args</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The connection string to connect to the test database.
+    <t>The connection string to connect to the test database.
 Use ";" to separate key/value pairs and "=" to separate the key from the value.
 Leading and trailing white spaces will be ignored for each key/value pair.
 Key names may be case sensitive (see database documentation).
 For a good overview over connection strings for different databases and drivers see:
 https://www.connectionstrings.com/
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Important:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Since the key/value pairs are converted into an R list (required by DBItest)
+Important: Since the key/value pairs are converted into an R list (required by DBItest)
 the values may not contain surrounding parenthesis (even if they contain spaces).
 This is the only difference to "real" connection strings.</t>
-    </r>
+  </si>
+  <si>
+    <t>OS.driver.name</t>
+  </si>
+  <si>
+    <t>The name of the database driver on the test client that is used by the connection string.
+This value is just for information purposes in the reports since different drivers and versions may behave differently.
+Normally you do only have to specify a value here if you are using ODBC or JDBC via DBI.
+The driver name of the operating system is the specified in the connection string as "DRIVER".
+In Windows you can find the driver names in the ODBC settings.
+In Linux you can find the driver (file) names in the config file with the shell command "cat /etc/odbcinst.ini" (check the correct name and path of the config file with "odbcinst -j").</t>
   </si>
   <si>
     <t>start.script</t>
@@ -191,21 +179,13 @@
     <t>driver=SQLite3; database=:memory:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Ubuntu Linux 14.04:
+    <t>libsqlite3odbc.so</t>
+  </si>
+  <si>
+    <t>Ubuntu Linux 14.04:
 sudo apt-get install libsqliteodbc
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R package:
+R package:
 install.packages("odbc")</t>
-    </r>
   </si>
   <si>
     <t>PostgreSQL Unicode with odbc driver</t>
@@ -214,27 +194,19 @@
     <t>driver=PostgreSQL Unicode;Database=postgres;Uid=postgres;Pwd=dbitesting;Server=localhost;Port=30000;</t>
   </si>
   <si>
+    <t>psqlodbcw.so</t>
+  </si>
+  <si>
     <t>start_postgres.sh</t>
   </si>
   <si>
     <t>stop_postgres.sh</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Ubuntu Linux 14.04:
+    <t>Ubuntu Linux 14.04:
 sudo apt-get install odbc-postgresql
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R package:
+R package:
 install.packages("odbc")</t>
-    </r>
   </si>
   <si>
     <t>Ubuntu: No need to create a DSN in odbc.ini (just the driver name is required and pre-installed in odbcinst.ini)</t>
@@ -262,37 +234,19 @@
     <t>driver = MySQL; server = 127.0.0.1; port = 30001; user = root; password=dbitesting; database = testdb; option=3; protocol = tcp;</t>
   </si>
   <si>
+    <t>libmyodbc.so</t>
+  </si>
+  <si>
     <t>start_mysql.sh</t>
   </si>
   <si>
     <t>stop_mysql.sh</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Ubuntu Linux 14.04:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">apt-get install libmyodbc
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R package:
+    <t>Ubuntu Linux 14.04:
+apt-get install libmyodbc
+R package:
 install.packages("odbc")</t>
-    </r>
   </si>
   <si>
     <t>For MySQL use 127.0.0.1 instead of "localhost" as server to switch from name Unix socket files to TCP protocol. See:
@@ -322,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -352,12 +306,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -415,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,10 +397,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -468,7 +412,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,10 +493,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -580,6 +524,11 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
+      <c r="B3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -598,7 +547,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -606,7 +555,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -614,7 +563,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -622,14 +571,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="128.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="72.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="162.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
@@ -637,33 +586,41 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+    <row r="12" customFormat="false" ht="72.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="43.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="43.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://www.connectionstrings.com/"/>
+    <hyperlink ref="B10" r:id="rId1" display="The connection string to connect to the test database.&#10;Use &quot;;&quot; to separate key/value pairs and &quot;=&quot; to separate the key from the value.&#10;Leading and trailing white spaces will be ignored for each key/value pair.&#10;Key names may be case sensitive (see database documentation).&#10;For a good overview over connection strings for different databases and drivers see:&#10;https://www.connectionstrings.com/&#10;Important: Since the key/value pairs are converted into an R list (required by DBItest)&#10;the values may not contain surrounding parenthesis (even if they contain spaces).&#10;This is the only difference to &quot;real&quot; connection strings."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -680,195 +637,213 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="12.9311740890688"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="34.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="20.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="21.6437246963563"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="51.5951417004049"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="18.1174089068826"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="38.3117408906883"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="49.7246963562753"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="12.9311740890688"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="34.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="20.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="21.6437246963563"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="51.5951417004049"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="9" width="18.1174089068826"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="38.3117408906883"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="9" width="49.7246963562753"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="9" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+    <row r="1" s="10" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>22</v>
       </c>
+      <c r="J1" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>30</v>
+      </c>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
-      <c r="B3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>35</v>
       </c>
+      <c r="E3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
-      <c r="B4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="I5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="C6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="43.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="I6" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="J6" s="9" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new version of comparative report
</commit_message>
<xml_diff>
--- a/test_configs.xlsx
+++ b/test_configs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>Purpose of this file:</t>
   </si>
@@ -640,7 +640,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -705,6 +705,7 @@
       <c r="E2" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
       <c r="I2" s="9" t="s">
@@ -715,7 +716,9 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
+      <c r="A3" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="B3" s="9" t="s">
         <v>33</v>
       </c>
@@ -739,7 +742,9 @@
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
+      <c r="A4" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="B4" s="9" t="s">
         <v>39</v>
       </c>
@@ -768,8 +773,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0"/>
+    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="B5" s="9" t="s">
         <v>46</v>
       </c>
@@ -782,6 +789,7 @@
       <c r="E5" s="9" t="s">
         <v>49</v>
       </c>
+      <c r="F5" s="0"/>
       <c r="G5" s="9" t="s">
         <v>42</v>
       </c>
@@ -794,7 +802,9 @@
       <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
+      <c r="A6" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
@@ -824,6 +834,9 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="B7" s="9" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Improved reports. Enabled all DBI tests incl. transactions (were blocking before)
</commit_message>
<xml_diff>
--- a/test_configs.xlsx
+++ b/test_configs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="293" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Purpose of this file:</t>
   </si>
@@ -496,7 +496,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -640,7 +640,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -689,7 +689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
@@ -715,10 +715,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>26</v>
-      </c>
+    <row r="3" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
       <c r="B3" s="9" t="s">
         <v>33</v>
       </c>
@@ -741,10 +739,8 @@
       </c>
       <c r="J3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>26</v>
-      </c>
+    <row r="4" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
       <c r="B4" s="9" t="s">
         <v>39</v>
       </c>
@@ -773,10 +769,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>26</v>
-      </c>
+    <row r="5" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
       <c r="B5" s="9" t="s">
         <v>46</v>
       </c>
@@ -801,10 +795,8 @@
       </c>
       <c r="J5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>26</v>
-      </c>
+    <row r="6" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
       <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
@@ -833,10 +825,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>26</v>
-      </c>
+    <row r="7" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9" t="s">
         <v>58</v>
       </c>

</xml_diff>